<commit_message>
att doc: legendas + bundown
</commit_message>
<xml_diff>
--- a/documentacao/BurnDown/burndownTerceiroSprint.xlsx
+++ b/documentacao/BurnDown/burndownTerceiroSprint.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\TCC\documentacao\BurnDown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32A05B9-256D-4841-BD60-8724CF38289A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CBF6075-DE3C-41BF-87DE-9233A63C3B3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
   <si>
     <t>Atividade 10</t>
   </si>
@@ -1109,9 +1109,16 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Planilha1!$B$18:$P$18</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Planilha1!$B$18:$L$18</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Planilha1!$B$18:$L$18</c:f>
               <c:strCache>
-                <c:ptCount val="15"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v> Total de horas</c:v>
                 </c:pt>
@@ -1144,66 +1151,55 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>Dia 10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Dia 11</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Dia 12</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Dia 13</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Dia 14</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$B$27:$P$27</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Planilha1!$B$27:$P$27</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Planilha1!$B$27:$L$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>77</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>58</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>49</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>39</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>36</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>32</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>30</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>26</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>12</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1249,9 +1245,16 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Planilha1!$B$18:$P$18</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Planilha1!$B$18:$L$18</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Planilha1!$B$18:$L$18</c:f>
               <c:strCache>
-                <c:ptCount val="15"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v> Total de horas</c:v>
                 </c:pt>
@@ -1284,71 +1287,54 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>Dia 10</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Dia 11</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Dia 12</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Dia 13</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Dia 14</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Planilha1!$B$28:$P$28</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Planilha1!$B$28:$P$28</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Planilha1!$B$28:$L$28</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>77</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>71.5</c:v>
+                  <c:v>67.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>66</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>60.5</c:v>
+                  <c:v>52.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>55</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>49.5</c:v>
+                  <c:v>37.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>44</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>38.5</c:v>
+                  <c:v>22.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>33</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>27.5</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>16.5</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>5.5</c:v>
-                </c:pt>
-                <c:pt idx="14">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -2684,15 +2670,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>3238499</xdr:colOff>
+      <xdr:colOff>3238500</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>138546</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>173181</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>467592</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2763,7 +2749,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -2815,7 +2801,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -3031,8 +3017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="P40" sqref="P40"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3814,7 +3800,7 @@
         <v>113</v>
       </c>
       <c r="D12" s="2">
-        <f t="shared" ref="C12:I12" si="0">IF(SUM(D2:D11)&gt;0,C12-SUM(D2:D11),"")</f>
+        <f t="shared" ref="D12:I12" si="0">IF(SUM(D2:D11)&gt;0,C12-SUM(D2:D11),"")</f>
         <v>105</v>
       </c>
       <c r="E12" s="2">
@@ -4014,18 +4000,10 @@
       <c r="L18" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M18" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="N18" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="O18" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="P18" s="6" t="s">
-        <v>15</v>
-      </c>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
       <c r="Q18" s="8"/>
       <c r="R18" s="8"/>
       <c r="S18" s="8"/>
@@ -4070,18 +4048,10 @@
       <c r="L19" s="4">
         <v>0</v>
       </c>
-      <c r="M19" s="4">
-        <v>0</v>
-      </c>
-      <c r="N19" s="4">
-        <v>0</v>
-      </c>
-      <c r="O19" s="4">
-        <v>0</v>
-      </c>
-      <c r="P19" s="4">
-        <v>0</v>
-      </c>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
       <c r="Q19" s="9"/>
       <c r="R19" s="9"/>
       <c r="S19" s="9"/>
@@ -4126,18 +4096,10 @@
       <c r="L20" s="4">
         <v>0</v>
       </c>
-      <c r="M20" s="4">
-        <v>0</v>
-      </c>
-      <c r="N20" s="4">
-        <v>0</v>
-      </c>
-      <c r="O20" s="4">
-        <v>0</v>
-      </c>
-      <c r="P20" s="4">
-        <v>0</v>
-      </c>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
       <c r="Q20" s="9"/>
       <c r="R20" s="9"/>
       <c r="S20" s="9"/>
@@ -4174,7 +4136,7 @@
         <v>0</v>
       </c>
       <c r="J21" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K21" s="4">
         <v>1</v>
@@ -4182,18 +4144,10 @@
       <c r="L21" s="4">
         <v>0</v>
       </c>
-      <c r="M21" s="4">
-        <v>1</v>
-      </c>
-      <c r="N21" s="4">
-        <v>0</v>
-      </c>
-      <c r="O21" s="4">
-        <v>0</v>
-      </c>
-      <c r="P21" s="4">
-        <v>0</v>
-      </c>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
       <c r="Q21" s="9"/>
       <c r="R21" s="9"/>
       <c r="S21" s="9"/>
@@ -4218,7 +4172,7 @@
         <v>0</v>
       </c>
       <c r="F22" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G22" s="4">
         <v>0</v>
@@ -4227,7 +4181,7 @@
         <v>0</v>
       </c>
       <c r="I22" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J22" s="4">
         <v>0</v>
@@ -4238,18 +4192,10 @@
       <c r="L22" s="4">
         <v>2</v>
       </c>
-      <c r="M22" s="4">
-        <v>1</v>
-      </c>
-      <c r="N22" s="4">
-        <v>2</v>
-      </c>
-      <c r="O22" s="4">
-        <v>1</v>
-      </c>
-      <c r="P22" s="4">
-        <v>0</v>
-      </c>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
       <c r="Q22" s="9"/>
       <c r="R22" s="9"/>
       <c r="S22" s="9"/>
@@ -4262,7 +4208,7 @@
         <v>39</v>
       </c>
       <c r="B23" s="4">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C23" s="4">
         <v>6</v>
@@ -4292,20 +4238,12 @@
         <v>0</v>
       </c>
       <c r="L23" s="4">
-        <v>1</v>
-      </c>
-      <c r="M23" s="4">
-        <v>0</v>
-      </c>
-      <c r="N23" s="4">
-        <v>1</v>
-      </c>
-      <c r="O23" s="4">
-        <v>0</v>
-      </c>
-      <c r="P23" s="4">
-        <v>0</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
       <c r="Q23" s="9"/>
       <c r="R23" s="9"/>
       <c r="S23" s="9"/>
@@ -4345,19 +4283,15 @@
         <v>0</v>
       </c>
       <c r="K24" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L24" s="4">
-        <v>0</v>
-      </c>
-      <c r="M24" s="4">
-        <v>0</v>
-      </c>
-      <c r="N24" s="4">
-        <v>0</v>
-      </c>
-      <c r="O24" s="4"/>
-      <c r="P24" s="4"/>
+        <v>2</v>
+      </c>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
       <c r="Q24" s="9"/>
       <c r="R24" s="9"/>
       <c r="S24" s="9"/>
@@ -4376,7 +4310,7 @@
         <v>0</v>
       </c>
       <c r="D25" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25" s="4">
         <v>0</v>
@@ -4391,10 +4325,10 @@
         <v>1</v>
       </c>
       <c r="I25" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J25" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K25" s="4">
         <v>2</v>
@@ -4402,18 +4336,10 @@
       <c r="L25" s="4">
         <v>0</v>
       </c>
-      <c r="M25" s="4">
-        <v>2</v>
-      </c>
-      <c r="N25" s="4">
-        <v>1</v>
-      </c>
-      <c r="O25" s="4">
-        <v>0</v>
-      </c>
-      <c r="P25" s="4">
-        <v>0</v>
-      </c>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
       <c r="Q25" s="9"/>
       <c r="R25" s="9"/>
       <c r="S25" s="9"/>
@@ -4456,20 +4382,12 @@
         <v>1</v>
       </c>
       <c r="L26" s="4">
-        <v>1</v>
-      </c>
-      <c r="M26" s="4">
-        <v>1</v>
-      </c>
-      <c r="N26" s="4">
-        <v>1</v>
-      </c>
-      <c r="O26" s="4">
-        <v>1</v>
-      </c>
-      <c r="P26" s="4">
-        <v>1</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="9"/>
       <c r="Q26" s="9"/>
       <c r="R26" s="9"/>
       <c r="S26" s="9"/>
@@ -4483,58 +4401,52 @@
       </c>
       <c r="B27" s="4">
         <f>SUM(B19:B26)</f>
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C27" s="4">
-        <f>IF(SUM(C19:C26)&gt;0,B27-SUM(C19:C26),"")</f>
-        <v>58</v>
+        <f t="shared" ref="C27:N27" si="9">IF(SUM(C19:C26)&gt;0,B27-SUM(C19:C26),"")</f>
+        <v>56</v>
       </c>
       <c r="D27" s="4">
-        <f>IF(SUM(D19:D26)&gt;0,C27-SUM(D19:D26),"")</f>
-        <v>49</v>
+        <f t="shared" si="9"/>
+        <v>48</v>
       </c>
       <c r="E27" s="4">
-        <f>IF(SUM(E19:E26)&gt;0,D27-SUM(E19:E26),"")</f>
-        <v>45</v>
+        <f t="shared" si="9"/>
+        <v>44</v>
       </c>
       <c r="F27" s="4">
-        <f>IF(SUM(F19:F26)&gt;0,E27-SUM(F19:F26),"")</f>
-        <v>42</v>
+        <f t="shared" si="9"/>
+        <v>39</v>
       </c>
       <c r="G27" s="4">
-        <f>IF(SUM(G19:G26)&gt;0,F27-SUM(G19:G26),"")</f>
-        <v>39</v>
+        <f t="shared" si="9"/>
+        <v>36</v>
       </c>
       <c r="H27" s="4">
-        <f>IF(SUM(H19:H26)&gt;0,G27-SUM(H19:H26),"")</f>
-        <v>36</v>
+        <f t="shared" si="9"/>
+        <v>33</v>
       </c>
       <c r="I27" s="4">
-        <f>IF(SUM(I19:I26)&gt;0,H27-SUM(I19:I26),"")</f>
-        <v>32</v>
+        <f t="shared" si="9"/>
+        <v>24</v>
       </c>
       <c r="J27" s="4">
-        <f>IF(SUM(J19:J26)&gt;0,I27-SUM(J19:J26),"")</f>
-        <v>30</v>
+        <f t="shared" si="9"/>
+        <v>20</v>
       </c>
       <c r="K27" s="4">
-        <f>IF(SUM(K19:K26)&gt;0,J27-SUM(K19:K26),"")</f>
-        <v>26</v>
+        <f t="shared" si="9"/>
+        <v>11</v>
       </c>
       <c r="L27" s="4">
-        <f>IF(SUM(L19:L26)&gt;0,K27-SUM(L19:L26),"")</f>
-        <v>22</v>
-      </c>
-      <c r="M27" s="4">
-        <f>IF(SUM(M19:M26)&gt;0,L27-SUM(M19:M26),"")</f>
-        <v>17</v>
-      </c>
-      <c r="N27" s="4">
-        <f>IF(SUM(N19:N26)&gt;0,M27-SUM(N19:N26),"")</f>
-        <v>12</v>
-      </c>
-      <c r="O27" s="4"/>
-      <c r="P27" s="4"/>
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9"/>
+      <c r="P27" s="9"/>
       <c r="Q27" s="9"/>
       <c r="R27" s="9"/>
       <c r="S27" s="9"/>
@@ -4548,64 +4460,52 @@
       </c>
       <c r="B28" s="4">
         <f>B27</f>
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C28" s="4">
         <f>B28-($B$28/COUNTA($C$18:$P$18))</f>
-        <v>71.5</v>
+        <v>67.5</v>
       </c>
       <c r="D28" s="4">
-        <f t="shared" ref="D28:P28" si="9">C28-($B$28/COUNTA($C$18:$P$18))</f>
-        <v>66</v>
+        <f t="shared" ref="D28:L28" si="10">C28-($B$28/COUNTA($C$18:$P$18))</f>
+        <v>60</v>
       </c>
       <c r="E28" s="4">
-        <f t="shared" si="9"/>
-        <v>60.5</v>
+        <f t="shared" si="10"/>
+        <v>52.5</v>
       </c>
       <c r="F28" s="4">
-        <f t="shared" si="9"/>
-        <v>55</v>
+        <f t="shared" si="10"/>
+        <v>45</v>
       </c>
       <c r="G28" s="4">
-        <f t="shared" si="9"/>
-        <v>49.5</v>
+        <f t="shared" si="10"/>
+        <v>37.5</v>
       </c>
       <c r="H28" s="4">
-        <f t="shared" si="9"/>
-        <v>44</v>
+        <f t="shared" si="10"/>
+        <v>30</v>
       </c>
       <c r="I28" s="4">
-        <f t="shared" si="9"/>
-        <v>38.5</v>
+        <f t="shared" si="10"/>
+        <v>22.5</v>
       </c>
       <c r="J28" s="4">
-        <f t="shared" si="9"/>
-        <v>33</v>
+        <f t="shared" si="10"/>
+        <v>15</v>
       </c>
       <c r="K28" s="4">
-        <f t="shared" si="9"/>
-        <v>27.5</v>
+        <f t="shared" si="10"/>
+        <v>7.5</v>
       </c>
       <c r="L28" s="4">
-        <f t="shared" si="9"/>
-        <v>22</v>
-      </c>
-      <c r="M28" s="4">
-        <f t="shared" si="9"/>
-        <v>16.5</v>
-      </c>
-      <c r="N28" s="4">
-        <f t="shared" si="9"/>
-        <v>11</v>
-      </c>
-      <c r="O28" s="4">
-        <f t="shared" si="9"/>
-        <v>5.5</v>
-      </c>
-      <c r="P28" s="4">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
       <c r="Q28" s="9"/>
       <c r="R28" s="9"/>
       <c r="S28" s="9"/>
@@ -4688,7 +4588,7 @@
     <row r="44" spans="22:22" x14ac:dyDescent="0.25">
       <c r="V44">
         <f>SUM(C24:U24)</f>
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="22:22" x14ac:dyDescent="0.25">
@@ -4700,13 +4600,13 @@
     <row r="47" spans="22:22" x14ac:dyDescent="0.25">
       <c r="V47">
         <f>SUM(C27:U27)</f>
-        <v>408</v>
+        <v>315</v>
       </c>
     </row>
     <row r="48" spans="22:22" x14ac:dyDescent="0.25">
       <c r="V48">
         <f>SUM(C28:U28)</f>
-        <v>500.5</v>
+        <v>337.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>